<commit_message>
Tune soc handling beyond 1
</commit_message>
<xml_diff>
--- a/SOC_Photon/Battery State/BattleBorn.xlsx
+++ b/SOC_Photon/Battery State/BattleBorn.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Coefficients Table" sheetId="7" r:id="rId1"/>
@@ -2167,11 +2167,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="436486072"/>
-        <c:axId val="436486464"/>
+        <c:axId val="669540448"/>
+        <c:axId val="669549464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="436486072"/>
+        <c:axId val="669540448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="90"/>
@@ -2219,7 +2219,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2286,12 +2285,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="436486464"/>
+        <c:crossAx val="669549464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="436486464"/>
+        <c:axId val="669549464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="13.1"/>
@@ -2339,7 +2338,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2406,7 +2404,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="436486072"/>
+        <c:crossAx val="669540448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -2421,7 +2419,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2528,6 +2525,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2862,11 +2860,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="442238920"/>
-        <c:axId val="442232648"/>
+        <c:axId val="566387928"/>
+        <c:axId val="566390280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="442238920"/>
+        <c:axId val="566387928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2924,12 +2922,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442232648"/>
+        <c:crossAx val="566390280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="442232648"/>
+        <c:axId val="566390280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="14"/>
@@ -2988,7 +2986,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442238920"/>
+        <c:crossAx val="566387928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -3003,6 +3001,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3459,11 +3458,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="442237744"/>
-        <c:axId val="442236176"/>
+        <c:axId val="566385968"/>
+        <c:axId val="566386752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="442237744"/>
+        <c:axId val="566385968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3521,12 +3520,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442236176"/>
+        <c:crossAx val="566386752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="442236176"/>
+        <c:axId val="566386752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="14"/>
@@ -3585,7 +3584,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442237744"/>
+        <c:crossAx val="566385968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -3600,6 +3599,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3711,6 +3711,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4048,11 +4049,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="442230688"/>
-        <c:axId val="442231080"/>
+        <c:axId val="667283400"/>
+        <c:axId val="667284576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="442230688"/>
+        <c:axId val="667283400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4110,12 +4111,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442231080"/>
+        <c:crossAx val="667284576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="442231080"/>
+        <c:axId val="667284576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="14"/>
@@ -4174,7 +4175,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442230688"/>
+        <c:crossAx val="667283400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -4189,6 +4190,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4300,6 +4302,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4637,11 +4640,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="442234608"/>
-        <c:axId val="442239704"/>
+        <c:axId val="667285752"/>
+        <c:axId val="667232440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="442234608"/>
+        <c:axId val="667285752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4699,12 +4702,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442239704"/>
+        <c:crossAx val="667232440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="442239704"/>
+        <c:axId val="667232440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="14"/>
@@ -4763,7 +4766,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442234608"/>
+        <c:crossAx val="667285752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -4778,6 +4781,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4884,6 +4888,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5239,11 +5244,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="442240488"/>
-        <c:axId val="442241664"/>
+        <c:axId val="667240672"/>
+        <c:axId val="667242632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="442240488"/>
+        <c:axId val="667240672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5300,7 +5305,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442241664"/>
+        <c:crossAx val="667242632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5308,7 +5313,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="442241664"/>
+        <c:axId val="667242632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5365,7 +5370,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442240488"/>
+        <c:crossAx val="667240672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5379,6 +5384,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5485,6 +5491,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5521,8 +5528,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.3627665120627045E-2"/>
-          <c:y val="6.3366703744901748E-2"/>
+          <c:x val="0.10216647790601517"/>
+          <c:y val="3.7411939191694478E-2"/>
           <c:w val="0.87420338510768347"/>
           <c:h val="0.68283832429733826"/>
         </c:manualLayout>
@@ -6451,14 +6458,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="442238136"/>
-        <c:axId val="442236568"/>
+        <c:axId val="667257528"/>
+        <c:axId val="667258704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="442238136"/>
+        <c:axId val="667257528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1"/>
+          <c:max val="1.1000000000000001"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -6513,16 +6520,16 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442236568"/>
+        <c:crossAx val="667258704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="442236568"/>
+        <c:axId val="667258704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="13.5"/>
-          <c:min val="10"/>
+          <c:max val="14.5"/>
+          <c:min val="9"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -6577,7 +6584,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442238136"/>
+        <c:crossAx val="667257528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6591,6 +6598,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6710,6 +6718,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7795,11 +7804,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="442232256"/>
-        <c:axId val="442242448"/>
+        <c:axId val="667252040"/>
+        <c:axId val="667268896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="442232256"/>
+        <c:axId val="667252040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -7921,13 +7930,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442242448"/>
+        <c:crossAx val="667268896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="442242448"/>
+        <c:axId val="667268896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="13.5"/>
@@ -7975,6 +7984,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8041,7 +8051,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442232256"/>
+        <c:crossAx val="667252040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8176,7 +8186,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9859,11 +9868,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="436487640"/>
-        <c:axId val="435205008"/>
+        <c:axId val="669560440"/>
+        <c:axId val="669580432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="436487640"/>
+        <c:axId val="669560440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="97.5"/>
@@ -9911,7 +9920,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9978,12 +9986,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="435205008"/>
+        <c:crossAx val="669580432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="435205008"/>
+        <c:axId val="669580432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -10030,7 +10038,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10097,7 +10104,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="436487640"/>
+        <c:crossAx val="669560440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10111,7 +10118,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10218,7 +10224,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11901,11 +11906,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="439037968"/>
-        <c:axId val="439038752"/>
+        <c:axId val="669582000"/>
+        <c:axId val="669583176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="439037968"/>
+        <c:axId val="669582000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -11953,7 +11958,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -12020,12 +12024,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="439038752"/>
+        <c:crossAx val="669583176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="439038752"/>
+        <c:axId val="669583176"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -12073,7 +12077,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -12140,7 +12143,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="439037968"/>
+        <c:crossAx val="669582000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12154,7 +12157,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12269,6 +12271,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13354,11 +13357,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="439039928"/>
-        <c:axId val="439040320"/>
+        <c:axId val="669483216"/>
+        <c:axId val="669486744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="439039928"/>
+        <c:axId val="669483216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -13480,13 +13483,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="439040320"/>
+        <c:crossAx val="669486744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="439040320"/>
+        <c:axId val="669486744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="13.5"/>
@@ -13534,6 +13537,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -13600,7 +13604,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="439039928"/>
+        <c:crossAx val="669483216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13730,6 +13734,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14677,11 +14682,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="439034832"/>
-        <c:axId val="439041496"/>
+        <c:axId val="669493408"/>
+        <c:axId val="669498504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="439034832"/>
+        <c:axId val="669493408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -14802,13 +14807,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="439041496"/>
+        <c:crossAx val="669498504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="439041496"/>
+        <c:axId val="669498504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="13.5"/>
@@ -14861,6 +14866,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -14927,7 +14933,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="439034832"/>
+        <c:crossAx val="669493408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15032,6 +15038,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15222,11 +15229,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="439036400"/>
-        <c:axId val="439041104"/>
+        <c:axId val="566404392"/>
+        <c:axId val="566399688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="439036400"/>
+        <c:axId val="566404392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15283,12 +15290,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="439041104"/>
+        <c:crossAx val="566399688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="439041104"/>
+        <c:axId val="566399688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15345,7 +15352,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="439036400"/>
+        <c:crossAx val="566404392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15434,6 +15441,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15756,11 +15764,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="439039144"/>
-        <c:axId val="439042280"/>
+        <c:axId val="566401256"/>
+        <c:axId val="566402432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="439039144"/>
+        <c:axId val="566401256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -15818,12 +15826,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="439042280"/>
+        <c:crossAx val="566402432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="439042280"/>
+        <c:axId val="566402432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="14.5"/>
@@ -15882,7 +15890,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="439039144"/>
+        <c:crossAx val="566401256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15896,6 +15904,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16007,6 +16016,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16344,11 +16354,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="439035224"/>
-        <c:axId val="439036792"/>
+        <c:axId val="566398512"/>
+        <c:axId val="566402824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="439035224"/>
+        <c:axId val="566398512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -16406,12 +16416,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="439036792"/>
+        <c:crossAx val="566402824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="439036792"/>
+        <c:axId val="566402824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="14"/>
@@ -16470,7 +16480,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="439035224"/>
+        <c:crossAx val="566398512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -16485,6 +16495,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16596,6 +16607,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16933,11 +16945,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="442235784"/>
-        <c:axId val="442231472"/>
+        <c:axId val="566403216"/>
+        <c:axId val="566396944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="442235784"/>
+        <c:axId val="566403216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -16995,12 +17007,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442231472"/>
+        <c:crossAx val="566396944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="442231472"/>
+        <c:axId val="566396944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="14"/>
@@ -17059,7 +17071,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442235784"/>
+        <c:crossAx val="566403216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -17074,6 +17086,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -26402,15 +26415,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>525780</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:colOff>441960</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>388620</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -26431,16 +26444,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>118110</xdr:rowOff>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -26461,16 +26474,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>118110</xdr:rowOff>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -26493,16 +26506,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>118110</xdr:rowOff>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -26525,16 +26538,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>118110</xdr:rowOff>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -26557,16 +26570,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>118110</xdr:rowOff>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -26589,16 +26602,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>118110</xdr:rowOff>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -26651,16 +26664,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>365760</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>548640</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -27001,9 +27014,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S10"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
@@ -30722,7 +30735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -31227,8 +31240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>